<commit_message>
add version3 FLK conv, move Cout loop into the kernel
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>parameters</t>
   </si>
@@ -69,10 +69,16 @@
     <t>amount</t>
   </si>
   <si>
+    <t>git version</t>
+  </si>
+  <si>
     <t>改回来了，在vgg测试</t>
   </si>
   <si>
     <t>vgg7</t>
+  </si>
+  <si>
+    <t>6a9aec0</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A5:L22"/>
+  <dimension ref="A5:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1059,6 +1065,7 @@
     <col min="8" max="9" width="11.375" customWidth="1"/>
     <col min="10" max="11" width="15.625" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:12">
@@ -1317,7 +1324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:14">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -1351,10 +1358,13 @@
       <c r="L18" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N18" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>64</v>
@@ -1375,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I19">
         <v>100</v>
@@ -1388,6 +1398,9 @@
       </c>
       <c r="L19">
         <v>0.0034</v>
+      </c>
+      <c r="N19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:12">
@@ -1410,7 +1423,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20">
         <v>1000</v>
@@ -1445,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I21">
         <v>1000</v>
@@ -1480,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I22">
         <v>1000</v>

</xml_diff>

<commit_message>
add v4 FLK, uniform Cout for masks, performance is close to MyConvolution
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>parameters</t>
   </si>
@@ -24,6 +24,9 @@
     <t>one conv time(s)</t>
   </si>
   <si>
+    <t>git version</t>
+  </si>
+  <si>
     <t>Cout</t>
   </si>
   <si>
@@ -57,9 +60,18 @@
     <t>FLKv2</t>
   </si>
   <si>
+    <t>FLKv3</t>
+  </si>
+  <si>
     <t>把v2里的im2col里的weight和mask改成常数</t>
   </si>
   <si>
+    <t>改回来了，加入v3</t>
+  </si>
+  <si>
+    <t>bb29928</t>
+  </si>
+  <si>
     <t>base_channel</t>
   </si>
   <si>
@@ -67,12 +79,6 @@
   </si>
   <si>
     <t>amount</t>
-  </si>
-  <si>
-    <t>git version</t>
-  </si>
-  <si>
-    <t>改回来了，在vgg测试</t>
   </si>
   <si>
     <t>vgg7</t>
@@ -1052,10 +1058,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A5:N22"/>
+  <dimension ref="A5:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1068,7 +1074,7 @@
     <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12">
+    <row r="5" spans="3:14">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,32 +1089,35 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="N5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="3:12">
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:12">
@@ -1211,36 +1220,39 @@
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="3:12">
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="3:12">
@@ -1274,7 +1286,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1304,7 +1316,10 @@
         <v>0.00215</v>
       </c>
     </row>
-    <row r="16" spans="3:8">
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
       <c r="C16">
         <v>16</v>
       </c>
@@ -1323,87 +1338,81 @@
       <c r="H16">
         <v>3</v>
       </c>
+      <c r="J16">
+        <v>0.0045</v>
+      </c>
+      <c r="K16">
+        <v>0.0213</v>
+      </c>
+      <c r="L16">
+        <v>0.0134</v>
+      </c>
+      <c r="M16">
+        <v>0.0126</v>
+      </c>
+      <c r="N16" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="18" spans="2:14">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="17" spans="3:14">
+      <c r="C17">
+        <v>256</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>128</v>
+      </c>
+      <c r="F17">
+        <v>112</v>
+      </c>
+      <c r="G17">
+        <v>112</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F19" t="s">
         <v>7</v>
       </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>64</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>112</v>
-      </c>
-      <c r="F19">
-        <v>112</v>
-      </c>
-      <c r="G19">
-        <v>3</v>
+      <c r="G19" t="s">
+        <v>8</v>
       </c>
       <c r="H19" t="s">
         <v>19</v>
       </c>
-      <c r="I19">
-        <v>100</v>
-      </c>
-      <c r="J19">
-        <v>0.0029</v>
-      </c>
-      <c r="K19">
-        <v>0.0046</v>
-      </c>
-      <c r="L19">
-        <v>0.0034</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="I19" t="s">
         <v>20</v>
       </c>
+      <c r="J19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:14">
       <c r="B20">
         <v>64</v>
       </c>
@@ -1423,22 +1432,25 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I20">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="J20">
-        <v>0.0068</v>
+        <v>0.0029</v>
       </c>
       <c r="K20">
-        <v>0.039</v>
+        <v>0.0046</v>
       </c>
       <c r="L20">
-        <v>0.028</v>
+        <v>0.0034</v>
+      </c>
+      <c r="N20" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:14">
       <c r="B21">
         <v>64</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>112</v>
@@ -1458,22 +1470,25 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I21">
         <v>1000</v>
       </c>
       <c r="J21">
-        <v>0.016</v>
+        <v>0.0068</v>
       </c>
       <c r="K21">
-        <v>0.619</v>
+        <v>0.039</v>
       </c>
       <c r="L21">
-        <v>0.439</v>
+        <v>0.028</v>
+      </c>
+      <c r="N21" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:14">
       <c r="B22">
         <v>64</v>
       </c>
@@ -1481,7 +1496,7 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E22">
         <v>112</v>
@@ -1493,19 +1508,60 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I22">
         <v>1000</v>
       </c>
       <c r="J22">
+        <v>0.016</v>
+      </c>
+      <c r="K22">
+        <v>0.619</v>
+      </c>
+      <c r="L22">
+        <v>0.439</v>
+      </c>
+      <c r="N22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>112</v>
+      </c>
+      <c r="F23">
+        <v>112</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23">
+        <v>1000</v>
+      </c>
+      <c r="J23">
         <v>0.011</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>0.304</v>
       </c>
-      <c r="L22">
+      <c r="L23">
         <v>0.218</v>
+      </c>
+      <c r="N23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full version of v4, still a little slower T_T
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
   <si>
     <t>parameters</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>bb29928</t>
+  </si>
+  <si>
+    <t>加入v4</t>
+  </si>
+  <si>
+    <t>22010a2</t>
   </si>
   <si>
     <t>base_channel</t>
@@ -1058,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A5:N23"/>
+  <dimension ref="A5:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1071,10 +1077,10 @@
     <col min="8" max="9" width="11.375" customWidth="1"/>
     <col min="10" max="11" width="15.625" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:14">
+    <row r="5" spans="3:15">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1095,7 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1316,7 +1322,7 @@
         <v>0.00215</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1350,11 +1356,11 @@
       <c r="M16">
         <v>0.0126</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="3:14">
+    <row r="17" spans="3:15">
       <c r="C17">
         <v>256</v>
       </c>
@@ -1373,84 +1379,102 @@
       <c r="H17">
         <v>3</v>
       </c>
-      <c r="N17" t="s">
+      <c r="J17">
+        <v>0.029</v>
+      </c>
+      <c r="K17">
+        <v>0.255</v>
+      </c>
+      <c r="L17">
+        <v>0.174</v>
+      </c>
+      <c r="M17">
+        <v>0.159</v>
+      </c>
+      <c r="O17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
-      <c r="B19" t="s">
+    <row r="18" spans="1:15">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C18">
+        <v>256</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>128</v>
+      </c>
+      <c r="F18">
+        <v>112</v>
+      </c>
+      <c r="G18">
+        <v>112</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>0.029</v>
+      </c>
+      <c r="K18">
+        <v>0.253</v>
+      </c>
+      <c r="L18">
+        <v>0.179</v>
+      </c>
+      <c r="M18">
+        <v>0.169</v>
+      </c>
+      <c r="N18">
+        <v>0.035</v>
+      </c>
+      <c r="O18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>6</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>8</v>
-      </c>
-      <c r="H19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20">
-        <v>64</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>112</v>
-      </c>
-      <c r="F20">
-        <v>112</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
       </c>
       <c r="H20" t="s">
         <v>21</v>
       </c>
-      <c r="I20">
-        <v>100</v>
-      </c>
-      <c r="J20">
-        <v>0.0029</v>
-      </c>
-      <c r="K20">
-        <v>0.0046</v>
-      </c>
-      <c r="L20">
-        <v>0.0034</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="I20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="2:14">
+      <c r="J20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
       <c r="B21">
         <v>64</v>
       </c>
@@ -1470,25 +1494,25 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I21">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="J21">
-        <v>0.0068</v>
+        <v>0.0029</v>
       </c>
       <c r="K21">
-        <v>0.039</v>
+        <v>0.0046</v>
       </c>
       <c r="L21">
-        <v>0.028</v>
-      </c>
-      <c r="N21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14">
+        <v>0.0034</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
       <c r="B22">
         <v>64</v>
       </c>
@@ -1496,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>112</v>
@@ -1508,25 +1532,25 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I22">
         <v>1000</v>
       </c>
       <c r="J22">
-        <v>0.016</v>
+        <v>0.0068</v>
       </c>
       <c r="K22">
-        <v>0.619</v>
+        <v>0.039</v>
       </c>
       <c r="L22">
-        <v>0.439</v>
-      </c>
-      <c r="N22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14">
+        <v>0.028</v>
+      </c>
+      <c r="O22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15">
       <c r="B23">
         <v>64</v>
       </c>
@@ -1534,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E23">
         <v>112</v>
@@ -1546,22 +1570,60 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I23">
         <v>1000</v>
       </c>
       <c r="J23">
+        <v>0.016</v>
+      </c>
+      <c r="K23">
+        <v>0.619</v>
+      </c>
+      <c r="L23">
+        <v>0.439</v>
+      </c>
+      <c r="O23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24">
+        <v>64</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>112</v>
+      </c>
+      <c r="F24">
+        <v>112</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>1000</v>
+      </c>
+      <c r="J24">
         <v>0.011</v>
       </c>
-      <c r="K23">
+      <c r="K24">
         <v>0.304</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <v>0.218</v>
       </c>
-      <c r="N23" t="s">
-        <v>22</v>
+      <c r="O24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>